<commit_message>
vault backup: 2023-12-08 17:08:17
Affected files:
0. Attach/0.5 Archives/Convergence.xlsx
1. Projects/2023-05-07 基于多智能体强化学习和反向拍卖机制的车联网任务调度/初稿-中文/2. 相关工作.md
1. Projects/2023-05-07 基于多智能体强化学习和反向拍卖机制的车联网任务调度/整合-英文/1. Introduction.md
1. Projects/2023-05-07 基于多智能体强化学习和反向拍卖机制的车联网任务调度/整合-英文/2. Related Works.md
1. Projects/2023-05-07 基于多智能体强化学习和反向拍卖机制的车联网任务调度/整合-英文/Corpus.md
1. Projects/Temp.md
</commit_message>
<xml_diff>
--- a/0. Attach/0.5 Archives/Convergence.xlsx
+++ b/0. Attach/0.5 Archives/Convergence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuming\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuany\Documents\MateNote\0. Attach\0.5 Archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB59787-3F2B-417A-B529-A89F695479F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A515FC-82F5-41AA-BCD5-535DAAC452CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17109" yWindow="6360" windowWidth="24635" windowHeight="11023" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPO" sheetId="1" r:id="rId1"/>
@@ -62,17 +62,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -98,12 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -163,7 +160,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -959,7 +956,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="669548736"/>
@@ -1018,7 +1015,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="103302448"/>
@@ -1059,7 +1056,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1084,67 +1081,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>强化学习方法的</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Mean Reward </a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2649,7 +2586,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="669506576"/>
@@ -2708,7 +2645,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1988922208"/>
@@ -2750,7 +2687,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2780,7 +2717,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4254,12 +4191,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4270,7 +4207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>40000</v>
       </c>
@@ -4281,7 +4218,7 @@
         <v>15219360</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>80000</v>
       </c>
@@ -4293,7 +4230,7 @@
         <v>16733755.24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>120000</v>
       </c>
@@ -4305,7 +4242,7 @@
         <v>16400023.449999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>160000</v>
       </c>
@@ -4317,7 +4254,7 @@
         <v>16221344.449999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>200000</v>
       </c>
@@ -4329,7 +4266,7 @@
         <v>16545797.539999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>240000</v>
       </c>
@@ -4341,7 +4278,7 @@
         <v>16410736.310000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>280000</v>
       </c>
@@ -4353,7 +4290,7 @@
         <v>16732687.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>320000</v>
       </c>
@@ -4365,7 +4302,7 @@
         <v>16733707.959999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>360000</v>
       </c>
@@ -4377,7 +4314,7 @@
         <v>16278236.08</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>400000</v>
       </c>
@@ -4389,7 +4326,7 @@
         <v>16668075.439999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>440000</v>
       </c>
@@ -4401,7 +4338,7 @@
         <v>16501184.92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>480000</v>
       </c>
@@ -4413,7 +4350,7 @@
         <v>16820697.25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>520000</v>
       </c>
@@ -4425,7 +4362,7 @@
         <v>17040746.25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>560000</v>
       </c>
@@ -4437,7 +4374,7 @@
         <v>16619414.470000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>600000</v>
       </c>
@@ -4449,7 +4386,7 @@
         <v>16651371.810000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>640000</v>
       </c>
@@ -4461,7 +4398,7 @@
         <v>16633188.709999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>680000</v>
       </c>
@@ -4473,7 +4410,7 @@
         <v>16022758.6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>720000</v>
       </c>
@@ -4485,7 +4422,7 @@
         <v>17046106.620000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>760000</v>
       </c>
@@ -4497,7 +4434,7 @@
         <v>16940875.129999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>800000</v>
       </c>
@@ -4509,7 +4446,7 @@
         <v>17031934.440000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>840000</v>
       </c>
@@ -4521,7 +4458,7 @@
         <v>16495650.205</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>880000</v>
       </c>
@@ -4533,7 +4470,7 @@
         <v>16831284.030000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>920000</v>
       </c>
@@ -4545,7 +4482,7 @@
         <v>16804017.259999998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>960000</v>
       </c>
@@ -4557,7 +4494,7 @@
         <v>16524759.91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>1000000</v>
       </c>
@@ -4569,7 +4506,7 @@
         <v>16866732.210000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>1040000</v>
       </c>
@@ -4581,7 +4518,7 @@
         <v>16819629.509999998</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>1080000</v>
       </c>
@@ -4593,7 +4530,7 @@
         <v>16808355.199999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>1120000</v>
       </c>
@@ -4605,7 +4542,7 @@
         <v>16586704.59</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>1160000</v>
       </c>
@@ -4617,7 +4554,7 @@
         <v>16980680.949999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>1200000</v>
       </c>
@@ -4629,7 +4566,7 @@
         <v>16870234.870000001</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>1240000</v>
       </c>
@@ -4641,7 +4578,7 @@
         <v>17006275.190000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>1280000</v>
       </c>
@@ -4653,7 +4590,7 @@
         <v>17248882.66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>1320000</v>
       </c>
@@ -4665,7 +4602,7 @@
         <v>17028386.469999999</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>1360000</v>
       </c>
@@ -4677,7 +4614,7 @@
         <v>17144366.280000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>1400000</v>
       </c>
@@ -4689,7 +4626,7 @@
         <v>16645396.799999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>1440000</v>
       </c>
@@ -4701,7 +4638,7 @@
         <v>17065002.859999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>1480000</v>
       </c>
@@ -4713,7 +4650,7 @@
         <v>16442973.390000001</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>1520000</v>
       </c>
@@ -4725,7 +4662,7 @@
         <v>16497735.449999999</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>1560000</v>
       </c>
@@ -4737,7 +4674,7 @@
         <v>16555411.140000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>1600000</v>
       </c>
@@ -4749,7 +4686,7 @@
         <v>16823863.039999999</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>1640000</v>
       </c>
@@ -4761,7 +4698,7 @@
         <v>16830454.66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>1680000</v>
       </c>
@@ -4773,7 +4710,7 @@
         <v>16806314.280000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>1720000</v>
       </c>
@@ -4785,7 +4722,7 @@
         <v>16999809.649999999</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>1760000</v>
       </c>
@@ -4797,7 +4734,7 @@
         <v>16744631.609999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>1800000</v>
       </c>
@@ -4809,7 +4746,7 @@
         <v>16918027.07</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>1840000</v>
       </c>
@@ -4821,7 +4758,7 @@
         <v>17033211</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>1880000</v>
       </c>
@@ -4833,7 +4770,7 @@
         <v>16574220.699999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>1920000</v>
       </c>
@@ -4845,7 +4782,7 @@
         <v>16990641.27</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>1960000</v>
       </c>
@@ -4857,7 +4794,7 @@
         <v>16612417.029999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>2000000</v>
       </c>
@@ -4869,7 +4806,7 @@
         <v>17283188.239999998</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>2040000</v>
       </c>
@@ -4881,7 +4818,7 @@
         <v>16544243.209999999</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>2080000</v>
       </c>
@@ -4893,7 +4830,7 @@
         <v>16781996.600000001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>2120000</v>
       </c>
@@ -4905,7 +4842,7 @@
         <v>17079419.32</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>2160000</v>
       </c>
@@ -4917,7 +4854,7 @@
         <v>16981689.59</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>2200000</v>
       </c>
@@ -4929,7 +4866,7 @@
         <v>16911277.850000001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>2240000</v>
       </c>
@@ -4941,7 +4878,7 @@
         <v>16933599.919999998</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>2280000</v>
       </c>
@@ -4953,7 +4890,7 @@
         <v>16632908.970000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>2320000</v>
       </c>
@@ -4965,7 +4902,7 @@
         <v>16363630.654999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>2360000</v>
       </c>
@@ -4977,7 +4914,7 @@
         <v>16925258.940000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>2400000</v>
       </c>
@@ -4989,7 +4926,7 @@
         <v>16867697.509999998</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>2440000</v>
       </c>
@@ -5001,7 +4938,7 @@
         <v>17029643.329999998</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>2480000</v>
       </c>
@@ -5013,7 +4950,7 @@
         <v>16914485.009999998</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>2520000</v>
       </c>
@@ -5025,7 +4962,7 @@
         <v>17003879.669999998</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>2560000</v>
       </c>
@@ -5037,7 +4974,7 @@
         <v>17063899.66</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>2600000</v>
       </c>
@@ -5049,7 +4986,7 @@
         <v>16957222.190000001</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>2640000</v>
       </c>
@@ -5061,7 +4998,7 @@
         <v>16822493.890000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>2680000</v>
       </c>
@@ -5073,7 +5010,7 @@
         <v>16989845.390000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>2720000</v>
       </c>
@@ -5085,7 +5022,7 @@
         <v>16701447.24</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>2760000</v>
       </c>
@@ -5097,7 +5034,7 @@
         <v>16528313.789999999</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>2800000</v>
       </c>
@@ -5109,7 +5046,7 @@
         <v>16740528.1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>2840000</v>
       </c>
@@ -5121,7 +5058,7 @@
         <v>16809208.210000001</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>2880000</v>
       </c>
@@ -5133,7 +5070,7 @@
         <v>16999441.259999998</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>2920000</v>
       </c>
@@ -5145,7 +5082,7 @@
         <v>16710538.789999999</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>2960000</v>
       </c>
@@ -5157,7 +5094,7 @@
         <v>16689243.09</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>3000000</v>
       </c>
@@ -5169,7 +5106,7 @@
         <v>16954174.600000001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>3040000</v>
       </c>
@@ -5181,7 +5118,7 @@
         <v>16874405.359999999</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>3080000</v>
       </c>
@@ -5193,7 +5130,7 @@
         <v>17046272.100000001</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>3120000</v>
       </c>
@@ -5205,7 +5142,7 @@
         <v>16943607.52</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
         <v>3160000</v>
       </c>
@@ -5217,7 +5154,7 @@
         <v>16680419.459999999</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>3200000</v>
       </c>
@@ -5229,7 +5166,7 @@
         <v>16510089.32</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>3240000</v>
       </c>
@@ -5241,7 +5178,7 @@
         <v>16683455.23</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>3280000</v>
       </c>
@@ -5253,7 +5190,7 @@
         <v>17298636.98</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>3320000</v>
       </c>
@@ -5265,7 +5202,7 @@
         <v>16764828.049999999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>3360000</v>
       </c>
@@ -5277,7 +5214,7 @@
         <v>17358580.140000001</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>3400000</v>
       </c>
@@ -5289,7 +5226,7 @@
         <v>16909315.73</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>3440000</v>
       </c>
@@ -5301,7 +5238,7 @@
         <v>16980432.73</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>3480000</v>
       </c>
@@ -5313,7 +5250,7 @@
         <v>16855962.219999999</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>3520000</v>
       </c>
@@ -5325,7 +5262,7 @@
         <v>16941934.989999998</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>3560000</v>
       </c>
@@ -5337,7 +5274,7 @@
         <v>16989402.140000001</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>3600000</v>
       </c>
@@ -5349,7 +5286,7 @@
         <v>16781655.789999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>3640000</v>
       </c>
@@ -5361,7 +5298,7 @@
         <v>17217563.600000001</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>3680000</v>
       </c>
@@ -5373,7 +5310,7 @@
         <v>17042176.469999999</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>3720000</v>
       </c>
@@ -5385,7 +5322,7 @@
         <v>16735679.93</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>3760000</v>
       </c>
@@ -5397,7 +5334,7 @@
         <v>16778740.190000001</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>3800000</v>
       </c>
@@ -5409,7 +5346,7 @@
         <v>17188634.149999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>3840000</v>
       </c>
@@ -5421,7 +5358,7 @@
         <v>17026723.789999999</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3">
       <c r="A98" s="1">
         <v>3880000</v>
       </c>
@@ -5433,7 +5370,7 @@
         <v>16922168.009999998</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3">
       <c r="A99" s="1">
         <v>3920000</v>
       </c>
@@ -5445,7 +5382,7 @@
         <v>16446987.265000001</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3">
       <c r="A100" s="1">
         <v>3960000</v>
       </c>
@@ -5457,7 +5394,7 @@
         <v>16540915.879999999</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3">
       <c r="A101" s="1">
         <v>4000000</v>
       </c>
@@ -5469,7 +5406,7 @@
         <v>17055749.77</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3">
       <c r="A102" s="1">
         <v>4040000</v>
       </c>
@@ -5481,7 +5418,7 @@
         <v>16890226.43</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3">
       <c r="A103" s="1">
         <v>4080000</v>
       </c>
@@ -5493,7 +5430,7 @@
         <v>16954883.800000001</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3">
       <c r="A104" s="1">
         <v>4120000</v>
       </c>
@@ -5505,7 +5442,7 @@
         <v>17038520.149999999</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3">
       <c r="A105" s="1">
         <v>4160000</v>
       </c>
@@ -5517,7 +5454,7 @@
         <v>16685852.720000001</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3">
       <c r="A106" s="1">
         <v>4200000</v>
       </c>
@@ -5529,7 +5466,7 @@
         <v>16937971.350000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3">
       <c r="A107" s="1">
         <v>4240000</v>
       </c>
@@ -5541,7 +5478,7 @@
         <v>16574994.91</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3">
       <c r="A108" s="1">
         <v>4280000</v>
       </c>
@@ -5553,7 +5490,7 @@
         <v>16820330.829999998</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3">
       <c r="A109" s="1">
         <v>4320000</v>
       </c>
@@ -5565,7 +5502,7 @@
         <v>17173392.259999998</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3">
       <c r="A110" s="1">
         <v>4360000</v>
       </c>
@@ -5577,7 +5514,7 @@
         <v>17143341.879999999</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3">
       <c r="A111" s="1">
         <v>4400000</v>
       </c>
@@ -5589,7 +5526,7 @@
         <v>16202174.379999999</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3">
       <c r="A112" s="1">
         <v>4440000</v>
       </c>
@@ -5601,7 +5538,7 @@
         <v>16707022.34</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3">
       <c r="A113" s="1">
         <v>4480000</v>
       </c>
@@ -5628,12 +5565,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5641,7 +5578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>40000</v>
       </c>
@@ -5649,7 +5586,7 @@
         <v>15329006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>80000</v>
       </c>
@@ -5657,7 +5594,7 @@
         <v>16610866</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>120000</v>
       </c>
@@ -5665,7 +5602,7 @@
         <v>16009182</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>160000</v>
       </c>
@@ -5673,7 +5610,7 @@
         <v>16770797</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>200000</v>
       </c>
@@ -5681,7 +5618,7 @@
         <v>16471980</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>240000</v>
       </c>
@@ -5689,7 +5626,7 @@
         <v>16475083</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
         <v>280000</v>
       </c>
@@ -5697,7 +5634,7 @@
         <v>16768047</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="1">
         <v>320000</v>
       </c>
@@ -5705,7 +5642,7 @@
         <v>17199456</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="1">
         <v>360000</v>
       </c>
@@ -5713,7 +5650,7 @@
         <v>16876734</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="1">
         <v>400000</v>
       </c>
@@ -5721,7 +5658,7 @@
         <v>17202868</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
         <v>440000</v>
       </c>
@@ -5729,7 +5666,7 @@
         <v>17128266</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
         <v>480000</v>
       </c>
@@ -5737,7 +5674,7 @@
         <v>17245810</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
         <v>520000</v>
       </c>
@@ -5745,7 +5682,7 @@
         <v>17099950</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
         <v>560000</v>
       </c>
@@ -5753,7 +5690,7 @@
         <v>17115842</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
         <v>600000</v>
       </c>
@@ -5761,7 +5698,7 @@
         <v>16920760</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>640000</v>
       </c>
@@ -5769,7 +5706,7 @@
         <v>17461166</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>680000</v>
       </c>
@@ -5777,7 +5714,7 @@
         <v>17005788</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>720000</v>
       </c>
@@ -5785,7 +5722,7 @@
         <v>17045452</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>760000</v>
       </c>
@@ -5793,7 +5730,7 @@
         <v>16878754</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>800000</v>
       </c>
@@ -5801,7 +5738,7 @@
         <v>16918552</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>840000</v>
       </c>
@@ -5809,7 +5746,7 @@
         <v>16912416</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>880000</v>
       </c>
@@ -5817,7 +5754,7 @@
         <v>17156170</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>920000</v>
       </c>
@@ -5825,7 +5762,7 @@
         <v>16929728</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>960000</v>
       </c>
@@ -5833,7 +5770,7 @@
         <v>17075106</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2">
       <c r="A26" s="1">
         <v>1000000</v>
       </c>
@@ -5841,7 +5778,7 @@
         <v>17350806</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2">
       <c r="A27" s="1">
         <v>1040000</v>
       </c>
@@ -5849,7 +5786,7 @@
         <v>17036966</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2">
       <c r="A28" s="1">
         <v>1080000</v>
       </c>
@@ -5857,7 +5794,7 @@
         <v>17161816</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>1120000</v>
       </c>
@@ -5865,7 +5802,7 @@
         <v>17488108</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
         <v>1160000</v>
       </c>
@@ -5873,7 +5810,7 @@
         <v>17459530</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
         <v>1200000</v>
       </c>
@@ -5881,7 +5818,7 @@
         <v>17233474</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2">
       <c r="A32" s="1">
         <v>1240000</v>
       </c>
@@ -5889,7 +5826,7 @@
         <v>16968440</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2">
       <c r="A33" s="1">
         <v>1280000</v>
       </c>
@@ -5897,7 +5834,7 @@
         <v>17108960</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2">
       <c r="A34" s="1">
         <v>1320000</v>
       </c>
@@ -5905,7 +5842,7 @@
         <v>17178824</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2">
       <c r="A35" s="1">
         <v>1360000</v>
       </c>
@@ -5913,7 +5850,7 @@
         <v>17300474</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2">
       <c r="A36" s="1">
         <v>1400000</v>
       </c>
@@ -5921,7 +5858,7 @@
         <v>17276922</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2">
       <c r="A37" s="1">
         <v>1440000</v>
       </c>
@@ -5929,7 +5866,7 @@
         <v>17022812</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2">
       <c r="A38" s="1">
         <v>1480000</v>
       </c>
@@ -5937,7 +5874,7 @@
         <v>16990642</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2">
       <c r="A39" s="1">
         <v>1520000</v>
       </c>
@@ -5945,7 +5882,7 @@
         <v>17303778</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2">
       <c r="A40" s="1">
         <v>1560000</v>
       </c>
@@ -5953,7 +5890,7 @@
         <v>16803994</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2">
       <c r="A41" s="1">
         <v>1600000</v>
       </c>
@@ -5961,7 +5898,7 @@
         <v>17278970</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2">
       <c r="A42" s="1">
         <v>1640000</v>
       </c>
@@ -5969,7 +5906,7 @@
         <v>17141988</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2">
       <c r="A43" s="1">
         <v>1680000</v>
       </c>
@@ -5977,7 +5914,7 @@
         <v>17099652</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2">
       <c r="A44" s="1">
         <v>1720000</v>
       </c>
@@ -5985,7 +5922,7 @@
         <v>17069394</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2">
       <c r="A45" s="1">
         <v>1760000</v>
       </c>
@@ -5993,7 +5930,7 @@
         <v>17355998</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2">
       <c r="A46" s="1">
         <v>1800000</v>
       </c>
@@ -6001,7 +5938,7 @@
         <v>17563594</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2">
       <c r="A47" s="1">
         <v>1840000</v>
       </c>
@@ -6009,7 +5946,7 @@
         <v>17010256</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2">
       <c r="A48" s="1">
         <v>1880000</v>
       </c>
@@ -6017,7 +5954,7 @@
         <v>17113982</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2">
       <c r="A49" s="1">
         <v>1920000</v>
       </c>
@@ -6025,7 +5962,7 @@
         <v>17345416</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2">
       <c r="A50" s="1">
         <v>1960000</v>
       </c>
@@ -6033,7 +5970,7 @@
         <v>17135978</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2">
       <c r="A51" s="1">
         <v>2000000</v>
       </c>
@@ -6041,7 +5978,7 @@
         <v>17091372</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2">
       <c r="A52" s="1">
         <v>2040000</v>
       </c>
@@ -6049,7 +5986,7 @@
         <v>17151396</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2">
       <c r="A53" s="1">
         <v>2080000</v>
       </c>
@@ -6057,7 +5994,7 @@
         <v>17390466</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2">
       <c r="A54" s="1">
         <v>2120000</v>
       </c>
@@ -6065,7 +6002,7 @@
         <v>17427718</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2">
       <c r="A55" s="1">
         <v>2160000</v>
       </c>
@@ -6073,7 +6010,7 @@
         <v>16830244</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2">
       <c r="A56" s="1">
         <v>2200000</v>
       </c>
@@ -6081,7 +6018,7 @@
         <v>17327410</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="A57" s="1">
         <v>2240000</v>
       </c>
@@ -6089,7 +6026,7 @@
         <v>17126952</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2">
       <c r="A58" s="1">
         <v>2280000</v>
       </c>
@@ -6097,7 +6034,7 @@
         <v>17327434</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2">
       <c r="A59" s="1">
         <v>2320000</v>
       </c>
@@ -6105,7 +6042,7 @@
         <v>17268976</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2">
       <c r="A60" s="1">
         <v>2360000</v>
       </c>
@@ -6113,7 +6050,7 @@
         <v>17096926</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2">
       <c r="A61" s="1">
         <v>2400000</v>
       </c>
@@ -6121,7 +6058,7 @@
         <v>17278970</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2">
       <c r="A62" s="1">
         <v>2440000</v>
       </c>
@@ -6129,7 +6066,7 @@
         <v>16855970</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2">
       <c r="A63" s="1">
         <v>2480000</v>
       </c>
@@ -6137,7 +6074,7 @@
         <v>17358912</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2">
       <c r="A64" s="1">
         <v>2520000</v>
       </c>
@@ -6145,7 +6082,7 @@
         <v>16908754</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2">
       <c r="A65" s="1">
         <v>2560000</v>
       </c>
@@ -6153,7 +6090,7 @@
         <v>17274282</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2">
       <c r="A66" s="1">
         <v>2600000</v>
       </c>
@@ -6161,7 +6098,7 @@
         <v>17237872</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2">
       <c r="A67" s="1">
         <v>2640000</v>
       </c>
@@ -6169,7 +6106,7 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2">
       <c r="A68" s="1">
         <v>2680000</v>
       </c>
@@ -6177,7 +6114,7 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2">
       <c r="A69" s="1">
         <v>2720000</v>
       </c>
@@ -6185,7 +6122,7 @@
         <v>17049062</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2">
       <c r="A70" s="1">
         <v>2760000</v>
       </c>
@@ -6193,7 +6130,7 @@
         <v>16856282</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2">
       <c r="A71" s="1">
         <v>2800000</v>
       </c>
@@ -6201,7 +6138,7 @@
         <v>17101702</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2">
       <c r="A72" s="1">
         <v>2840000</v>
       </c>
@@ -6209,7 +6146,7 @@
         <v>17278706</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2">
       <c r="A73" s="1">
         <v>2880000</v>
       </c>
@@ -6217,7 +6154,7 @@
         <v>16938186</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2">
       <c r="A74" s="1">
         <v>2920000</v>
       </c>
@@ -6225,7 +6162,7 @@
         <v>16873510</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2">
       <c r="A75" s="1">
         <v>2960000</v>
       </c>
@@ -6233,7 +6170,7 @@
         <v>17593932</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2">
       <c r="A76" s="1">
         <v>3000000</v>
       </c>
@@ -6241,7 +6178,7 @@
         <v>17134430</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2">
       <c r="A77" s="1">
         <v>3040000</v>
       </c>
@@ -6249,7 +6186,7 @@
         <v>17164636</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2">
       <c r="A78" s="1">
         <v>3080000</v>
       </c>
@@ -6257,7 +6194,7 @@
         <v>16973108</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2">
       <c r="A79" s="1">
         <v>3120000</v>
       </c>
@@ -6265,7 +6202,7 @@
         <v>17021286</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2">
       <c r="A80" s="1">
         <v>3160000</v>
       </c>
@@ -6273,7 +6210,7 @@
         <v>17230620</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2">
       <c r="A81" s="1">
         <v>3200000</v>
       </c>
@@ -6281,7 +6218,7 @@
         <v>17593932</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2">
       <c r="A82" s="1">
         <v>3240000</v>
       </c>
@@ -6289,7 +6226,7 @@
         <v>17134430</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2">
       <c r="A83" s="1">
         <v>3280000</v>
       </c>
@@ -6297,7 +6234,7 @@
         <v>17164636</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2">
       <c r="A84" s="1">
         <v>3320000</v>
       </c>
@@ -6305,7 +6242,7 @@
         <v>17104460</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2">
       <c r="A85" s="1">
         <v>3360000</v>
       </c>
@@ -6313,7 +6250,7 @@
         <v>17137554</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2">
       <c r="A86" s="1">
         <v>3400000</v>
       </c>
@@ -6321,7 +6258,7 @@
         <v>17341466</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2">
       <c r="A87" s="1">
         <v>3440000</v>
       </c>
@@ -6329,7 +6266,7 @@
         <v>17361898</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2">
       <c r="A88" s="1">
         <v>3480000</v>
       </c>
@@ -6337,7 +6274,7 @@
         <v>17048576</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2">
       <c r="A89" s="1">
         <v>3520000</v>
       </c>
@@ -6345,7 +6282,7 @@
         <v>17090088</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2">
       <c r="A90" s="1">
         <v>3560000</v>
       </c>
@@ -6353,7 +6290,7 @@
         <v>17365918</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2">
       <c r="A91" s="1">
         <v>3600000</v>
       </c>
@@ -6361,7 +6298,7 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2">
       <c r="A92" s="1">
         <v>3640000</v>
       </c>
@@ -6369,7 +6306,7 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2">
       <c r="A93" s="1">
         <v>3680000</v>
       </c>
@@ -6377,7 +6314,7 @@
         <v>17049062</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2">
       <c r="A94" s="1">
         <v>3720000</v>
       </c>
@@ -6385,7 +6322,7 @@
         <v>17557028</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2">
       <c r="A95" s="1">
         <v>3760000</v>
       </c>
@@ -6393,7 +6330,7 @@
         <v>17205320</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2">
       <c r="A96" s="1">
         <v>3800000</v>
       </c>
@@ -6401,7 +6338,7 @@
         <v>17563594</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2">
       <c r="A97" s="1">
         <v>3840000</v>
       </c>
@@ -6409,7 +6346,7 @@
         <v>17010256</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2">
       <c r="A98" s="1">
         <v>3880000</v>
       </c>
@@ -6417,7 +6354,7 @@
         <v>17113982</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2">
       <c r="A99" s="1">
         <v>3920000</v>
       </c>
@@ -6425,7 +6362,7 @@
         <v>17266488</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2">
       <c r="A100" s="1">
         <v>3960000</v>
       </c>
@@ -6433,7 +6370,7 @@
         <v>17150440</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2">
       <c r="A101" s="1">
         <v>4000000</v>
       </c>
@@ -6441,7 +6378,7 @@
         <v>17230104</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2">
       <c r="A102" s="1">
         <v>4040000</v>
       </c>
@@ -6449,7 +6386,7 @@
         <v>17220920</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2">
       <c r="A103" s="1">
         <v>4080000</v>
       </c>
@@ -6457,7 +6394,7 @@
         <v>17133253</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2">
       <c r="A104" s="1">
         <v>4120000</v>
       </c>
@@ -6465,7 +6402,7 @@
         <v>17400828</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2">
       <c r="A105" s="1">
         <v>4160000</v>
       </c>
@@ -6473,7 +6410,7 @@
         <v>17048576</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2">
       <c r="A106" s="1">
         <v>4200000</v>
       </c>
@@ -6481,7 +6418,7 @@
         <v>17090088</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2">
       <c r="A107" s="1">
         <v>4240000</v>
       </c>
@@ -6489,7 +6426,7 @@
         <v>17365918</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2">
       <c r="A108" s="1">
         <v>4280000</v>
       </c>
@@ -6497,7 +6434,7 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2">
       <c r="A109" s="1">
         <v>4320000</v>
       </c>
@@ -6505,7 +6442,7 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2">
       <c r="A110" s="1">
         <v>4360000</v>
       </c>
@@ -6513,7 +6450,7 @@
         <v>17030244</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2">
       <c r="A111" s="1">
         <v>4400000</v>
       </c>
@@ -6521,7 +6458,7 @@
         <v>17327410</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2">
       <c r="A112" s="1">
         <v>4440000</v>
       </c>
@@ -6529,7 +6466,7 @@
         <v>17126952</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2">
       <c r="A113" s="1">
         <v>4480000</v>
       </c>
@@ -6549,18 +6486,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1D7311-1418-4A4F-A7C3-69519B136378}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6570,8 +6506,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
         <v>40000</v>
       </c>
       <c r="B2" s="1">
@@ -6581,8 +6517,8 @@
         <v>15329006</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
         <v>80000</v>
       </c>
       <c r="B3" s="1">
@@ -6592,8 +6528,8 @@
         <v>16610866</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>120000</v>
       </c>
       <c r="B4" s="1">
@@ -6603,8 +6539,8 @@
         <v>16009182</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>160000</v>
       </c>
       <c r="B5" s="1">
@@ -6614,8 +6550,8 @@
         <v>16770797</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
         <v>200000</v>
       </c>
       <c r="B6" s="1">
@@ -6625,8 +6561,8 @@
         <v>16471980</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
         <v>240000</v>
       </c>
       <c r="B7" s="1">
@@ -6636,8 +6572,8 @@
         <v>16475083</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>280000</v>
       </c>
       <c r="B8" s="1">
@@ -6647,8 +6583,8 @@
         <v>16768047</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>320000</v>
       </c>
       <c r="B9" s="1">
@@ -6658,8 +6594,8 @@
         <v>17199456</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>360000</v>
       </c>
       <c r="B10" s="1">
@@ -6669,8 +6605,8 @@
         <v>16876734</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
         <v>400000</v>
       </c>
       <c r="B11" s="1">
@@ -6680,8 +6616,8 @@
         <v>17202868</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
         <v>440000</v>
       </c>
       <c r="B12" s="1">
@@ -6691,8 +6627,8 @@
         <v>17128266</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
         <v>480000</v>
       </c>
       <c r="B13" s="1">
@@ -6702,8 +6638,8 @@
         <v>17245810</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
         <v>520000</v>
       </c>
       <c r="B14" s="1">
@@ -6713,8 +6649,8 @@
         <v>17099950</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
         <v>560000</v>
       </c>
       <c r="B15" s="1">
@@ -6724,8 +6660,8 @@
         <v>17115842</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
         <v>600000</v>
       </c>
       <c r="B16" s="1">
@@ -6735,8 +6671,8 @@
         <v>16920760</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
         <v>640000</v>
       </c>
       <c r="B17" s="1">
@@ -6746,8 +6682,8 @@
         <v>17461166</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
         <v>680000</v>
       </c>
       <c r="B18" s="1">
@@ -6757,8 +6693,8 @@
         <v>17005788</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
         <v>720000</v>
       </c>
       <c r="B19" s="1">
@@ -6768,8 +6704,8 @@
         <v>17045452</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>760000</v>
       </c>
       <c r="B20" s="1">
@@ -6779,8 +6715,8 @@
         <v>16878754</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
         <v>800000</v>
       </c>
       <c r="B21" s="1">
@@ -6790,8 +6726,8 @@
         <v>16918552</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
         <v>840000</v>
       </c>
       <c r="B22" s="1">
@@ -6801,8 +6737,8 @@
         <v>16912416</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
         <v>880000</v>
       </c>
       <c r="B23" s="1">
@@ -6812,8 +6748,8 @@
         <v>17156170</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
         <v>920000</v>
       </c>
       <c r="B24" s="1">
@@ -6823,8 +6759,8 @@
         <v>16929728</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
         <v>960000</v>
       </c>
       <c r="B25" s="1">
@@ -6834,8 +6770,8 @@
         <v>17075106</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
         <v>1000000</v>
       </c>
       <c r="B26" s="1">
@@ -6845,8 +6781,8 @@
         <v>17350806</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
         <v>1040000</v>
       </c>
       <c r="B27" s="1">
@@ -6856,8 +6792,8 @@
         <v>17036966</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
         <v>1080000</v>
       </c>
       <c r="B28" s="1">
@@ -6867,8 +6803,8 @@
         <v>17161816</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
         <v>1120000</v>
       </c>
       <c r="B29" s="1">
@@ -6878,8 +6814,8 @@
         <v>17488108</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
         <v>1160000</v>
       </c>
       <c r="B30" s="1">
@@ -6889,8 +6825,8 @@
         <v>17459530</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
         <v>1200000</v>
       </c>
       <c r="B31" s="1">
@@ -6900,8 +6836,8 @@
         <v>17233474</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
         <v>1240000</v>
       </c>
       <c r="B32" s="1">
@@ -6911,8 +6847,8 @@
         <v>16968440</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
         <v>1280000</v>
       </c>
       <c r="B33" s="1">
@@ -6922,8 +6858,8 @@
         <v>17108960</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
         <v>1320000</v>
       </c>
       <c r="B34" s="1">
@@ -6933,8 +6869,8 @@
         <v>17178824</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
         <v>1360000</v>
       </c>
       <c r="B35" s="1">
@@ -6944,8 +6880,8 @@
         <v>17300474</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
         <v>1400000</v>
       </c>
       <c r="B36" s="1">
@@ -6955,8 +6891,8 @@
         <v>17276922</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
         <v>1440000</v>
       </c>
       <c r="B37" s="1">
@@ -6966,8 +6902,8 @@
         <v>17022812</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
         <v>1480000</v>
       </c>
       <c r="B38" s="1">
@@ -6977,8 +6913,8 @@
         <v>16990642</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
         <v>1520000</v>
       </c>
       <c r="B39" s="1">
@@ -6988,8 +6924,8 @@
         <v>17303778</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
         <v>1560000</v>
       </c>
       <c r="B40" s="1">
@@ -6999,8 +6935,8 @@
         <v>16803994</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
         <v>1600000</v>
       </c>
       <c r="B41" s="1">
@@ -7010,8 +6946,8 @@
         <v>17278970</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
         <v>1640000</v>
       </c>
       <c r="B42" s="1">
@@ -7021,8 +6957,8 @@
         <v>17141988</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
         <v>1680000</v>
       </c>
       <c r="B43" s="1">
@@ -7032,8 +6968,8 @@
         <v>17099652</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
         <v>1720000</v>
       </c>
       <c r="B44" s="1">
@@ -7043,8 +6979,8 @@
         <v>17069394</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
         <v>1760000</v>
       </c>
       <c r="B45" s="1">
@@ -7054,8 +6990,8 @@
         <v>17355998</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
         <v>1800000</v>
       </c>
       <c r="B46" s="1">
@@ -7065,8 +7001,8 @@
         <v>17563594</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
         <v>1840000</v>
       </c>
       <c r="B47" s="1">
@@ -7076,8 +7012,8 @@
         <v>17010256</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
         <v>1880000</v>
       </c>
       <c r="B48" s="1">
@@ -7087,8 +7023,8 @@
         <v>17113982</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
         <v>1920000</v>
       </c>
       <c r="B49" s="1">
@@ -7098,8 +7034,8 @@
         <v>17345416</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
         <v>1960000</v>
       </c>
       <c r="B50" s="1">
@@ -7109,8 +7045,8 @@
         <v>17135978</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
         <v>2000000</v>
       </c>
       <c r="B51" s="1">
@@ -7120,8 +7056,8 @@
         <v>17091372</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
         <v>2040000</v>
       </c>
       <c r="B52" s="1">
@@ -7131,8 +7067,8 @@
         <v>17151396</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
         <v>2080000</v>
       </c>
       <c r="B53" s="1">
@@ -7142,8 +7078,8 @@
         <v>17390466</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="2">
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
         <v>2120000</v>
       </c>
       <c r="B54" s="1">
@@ -7153,8 +7089,8 @@
         <v>17427718</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="2">
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
         <v>2160000</v>
       </c>
       <c r="B55" s="1">
@@ -7164,8 +7100,8 @@
         <v>16830244</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
         <v>2200000</v>
       </c>
       <c r="B56" s="1">
@@ -7175,8 +7111,8 @@
         <v>17327410</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="2">
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
         <v>2240000</v>
       </c>
       <c r="B57" s="1">
@@ -7186,8 +7122,8 @@
         <v>17126952</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="2">
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
         <v>2280000</v>
       </c>
       <c r="B58" s="1">
@@ -7197,8 +7133,8 @@
         <v>17327434</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="2">
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
         <v>2320000</v>
       </c>
       <c r="B59" s="1">
@@ -7208,8 +7144,8 @@
         <v>17268976</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="2">
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
         <v>2360000</v>
       </c>
       <c r="B60" s="1">
@@ -7219,8 +7155,8 @@
         <v>17096926</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="2">
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
         <v>2400000</v>
       </c>
       <c r="B61" s="1">
@@ -7230,8 +7166,8 @@
         <v>17278970</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
         <v>2440000</v>
       </c>
       <c r="B62" s="1">
@@ -7241,8 +7177,8 @@
         <v>16855970</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="2">
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
         <v>2480000</v>
       </c>
       <c r="B63" s="1">
@@ -7252,8 +7188,8 @@
         <v>17358912</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="2">
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
         <v>2520000</v>
       </c>
       <c r="B64" s="1">
@@ -7263,8 +7199,8 @@
         <v>16908754</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="2">
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
         <v>2560000</v>
       </c>
       <c r="B65" s="1">
@@ -7274,8 +7210,8 @@
         <v>17274282</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="2">
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
         <v>2600000</v>
       </c>
       <c r="B66" s="1">
@@ -7285,8 +7221,8 @@
         <v>17237872</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="2">
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
         <v>2640000</v>
       </c>
       <c r="B67" s="1">
@@ -7296,8 +7232,8 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="2">
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
         <v>2680000</v>
       </c>
       <c r="B68" s="1">
@@ -7307,8 +7243,8 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="2">
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
         <v>2720000</v>
       </c>
       <c r="B69" s="1">
@@ -7318,8 +7254,8 @@
         <v>17049062</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="2">
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
         <v>2760000</v>
       </c>
       <c r="B70" s="1">
@@ -7329,8 +7265,8 @@
         <v>16856282</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="2">
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
         <v>2800000</v>
       </c>
       <c r="B71" s="1">
@@ -7340,8 +7276,8 @@
         <v>17101702</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="2">
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
         <v>2840000</v>
       </c>
       <c r="B72" s="1">
@@ -7351,8 +7287,8 @@
         <v>17278706</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="2">
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
         <v>2880000</v>
       </c>
       <c r="B73" s="1">
@@ -7362,8 +7298,8 @@
         <v>16938186</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="2">
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
         <v>2920000</v>
       </c>
       <c r="B74" s="1">
@@ -7373,8 +7309,8 @@
         <v>16873510</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="2">
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
         <v>2960000</v>
       </c>
       <c r="B75" s="1">
@@ -7384,8 +7320,8 @@
         <v>17593932</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="2">
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
         <v>3000000</v>
       </c>
       <c r="B76" s="1">
@@ -7395,8 +7331,8 @@
         <v>17134430</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="2">
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
         <v>3040000</v>
       </c>
       <c r="B77" s="1">
@@ -7406,8 +7342,8 @@
         <v>17164636</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="2">
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
         <v>3080000</v>
       </c>
       <c r="B78" s="1">
@@ -7417,8 +7353,8 @@
         <v>16973108</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="2">
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
         <v>3120000</v>
       </c>
       <c r="B79" s="1">
@@ -7428,8 +7364,8 @@
         <v>17021286</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="2">
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
         <v>3160000</v>
       </c>
       <c r="B80" s="1">
@@ -7439,8 +7375,8 @@
         <v>17230620</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="2">
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
         <v>3200000</v>
       </c>
       <c r="B81" s="1">
@@ -7450,8 +7386,8 @@
         <v>17593932</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="2">
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
         <v>3240000</v>
       </c>
       <c r="B82" s="1">
@@ -7461,8 +7397,8 @@
         <v>17134430</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="2">
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
         <v>3280000</v>
       </c>
       <c r="B83" s="1">
@@ -7472,8 +7408,8 @@
         <v>17164636</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="2">
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
         <v>3320000</v>
       </c>
       <c r="B84" s="1">
@@ -7483,8 +7419,8 @@
         <v>17104460</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="2">
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
         <v>3360000</v>
       </c>
       <c r="B85" s="1">
@@ -7494,8 +7430,8 @@
         <v>17137554</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="2">
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
         <v>3400000</v>
       </c>
       <c r="B86" s="1">
@@ -7505,8 +7441,8 @@
         <v>17341466</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="2">
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
         <v>3440000</v>
       </c>
       <c r="B87" s="1">
@@ -7516,8 +7452,8 @@
         <v>17361898</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="2">
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
         <v>3480000</v>
       </c>
       <c r="B88" s="1">
@@ -7527,8 +7463,8 @@
         <v>17048576</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="2">
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
         <v>3520000</v>
       </c>
       <c r="B89" s="1">
@@ -7538,8 +7474,8 @@
         <v>17090088</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="2">
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
         <v>3560000</v>
       </c>
       <c r="B90" s="1">
@@ -7549,8 +7485,8 @@
         <v>17365918</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="2">
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
         <v>3600000</v>
       </c>
       <c r="B91" s="1">
@@ -7560,8 +7496,8 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="2">
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
         <v>3640000</v>
       </c>
       <c r="B92" s="1">
@@ -7571,8 +7507,8 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="2">
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
         <v>3680000</v>
       </c>
       <c r="B93" s="1">
@@ -7582,8 +7518,8 @@
         <v>17049062</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="2">
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
         <v>3720000</v>
       </c>
       <c r="B94" s="1">
@@ -7593,8 +7529,8 @@
         <v>17557028</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="2">
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
         <v>3760000</v>
       </c>
       <c r="B95" s="1">
@@ -7604,8 +7540,8 @@
         <v>17205320</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="2">
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
         <v>3800000</v>
       </c>
       <c r="B96" s="1">
@@ -7615,8 +7551,8 @@
         <v>17563594</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="2">
+    <row r="97" spans="1:3">
+      <c r="A97" s="1">
         <v>3840000</v>
       </c>
       <c r="B97" s="1">
@@ -7626,8 +7562,8 @@
         <v>17010256</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="2">
+    <row r="98" spans="1:3">
+      <c r="A98" s="1">
         <v>3880000</v>
       </c>
       <c r="B98" s="1">
@@ -7637,8 +7573,8 @@
         <v>17113982</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="2">
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
         <v>3920000</v>
       </c>
       <c r="B99" s="1">
@@ -7648,8 +7584,8 @@
         <v>17266488</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="2">
+    <row r="100" spans="1:3">
+      <c r="A100" s="1">
         <v>3960000</v>
       </c>
       <c r="B100" s="1">
@@ -7659,8 +7595,8 @@
         <v>17150440</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="2">
+    <row r="101" spans="1:3">
+      <c r="A101" s="1">
         <v>4000000</v>
       </c>
       <c r="B101" s="1">
@@ -7670,8 +7606,8 @@
         <v>17230104</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="2">
+    <row r="102" spans="1:3">
+      <c r="A102" s="1">
         <v>4040000</v>
       </c>
       <c r="B102" s="1">
@@ -7681,8 +7617,8 @@
         <v>17220920</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="2">
+    <row r="103" spans="1:3">
+      <c r="A103" s="1">
         <v>4080000</v>
       </c>
       <c r="B103" s="1">
@@ -7692,8 +7628,8 @@
         <v>17133253</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="2">
+    <row r="104" spans="1:3">
+      <c r="A104" s="1">
         <v>4120000</v>
       </c>
       <c r="B104" s="1">
@@ -7703,8 +7639,8 @@
         <v>17400828</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="2">
+    <row r="105" spans="1:3">
+      <c r="A105" s="1">
         <v>4160000</v>
       </c>
       <c r="B105" s="1">
@@ -7714,8 +7650,8 @@
         <v>17248576</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="2">
+    <row r="106" spans="1:3">
+      <c r="A106" s="1">
         <v>4200000</v>
       </c>
       <c r="B106" s="1">
@@ -7725,8 +7661,8 @@
         <v>17090088</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="2">
+    <row r="107" spans="1:3">
+      <c r="A107" s="1">
         <v>4240000</v>
       </c>
       <c r="B107" s="1">
@@ -7736,8 +7672,8 @@
         <v>17365918</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="2">
+    <row r="108" spans="1:3">
+      <c r="A108" s="1">
         <v>4280000</v>
       </c>
       <c r="B108" s="1">
@@ -7747,8 +7683,8 @@
         <v>17036292</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="2">
+    <row r="109" spans="1:3">
+      <c r="A109" s="1">
         <v>4320000</v>
       </c>
       <c r="B109" s="1">
@@ -7758,8 +7694,8 @@
         <v>17154496</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="2">
+    <row r="110" spans="1:3">
+      <c r="A110" s="1">
         <v>4360000</v>
       </c>
       <c r="B110" s="1">
@@ -7769,8 +7705,8 @@
         <v>17030244</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="2">
+    <row r="111" spans="1:3">
+      <c r="A111" s="1">
         <v>4400000</v>
       </c>
       <c r="B111" s="1">
@@ -7780,8 +7716,8 @@
         <v>17327410</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="2">
+    <row r="112" spans="1:3">
+      <c r="A112" s="1">
         <v>4440000</v>
       </c>
       <c r="B112" s="1">
@@ -7791,8 +7727,8 @@
         <v>17126952</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="2">
+    <row r="113" spans="1:3">
+      <c r="A113" s="1">
         <v>4480000</v>
       </c>
       <c r="B113" s="1">
@@ -7802,7 +7738,7 @@
         <v>17327434</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3">
       <c r="B114" s="1">
         <f>AVERAGE(B99:B113)</f>
         <v>16797302.777666662</v>
@@ -7812,7 +7748,7 @@
         <v>17207296.199999999</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3">
       <c r="B115" s="1">
         <f>_xlfn.STDEV.P(B99:B113)</f>
         <v>264912.5059648804</v>
@@ -7835,10 +7771,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C49"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>